<commit_message>
Added in an invert drive command to robot teleop, cleanup in all VI's, altered motor jog mode a little, made swerve Teleop more modular, added more features to the double joystick method and swapped some control layouts around, removed useless code in periodic tasks, Fixed the front panels of global data and controlMain to actually be readable, and put comments everywhere.
</commit_message>
<xml_diff>
--- a/Team 34 Code/Robot Control Layout.xlsx
+++ b/Team 34 Code/Robot Control Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Coleman Cook\Documents\LabVIEW Data\2017 Robot Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Coleman Cook\Documents\LabVIEW Data\2017 Robot Project\Team 34 Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Mechanism</t>
   </si>
@@ -101,9 +101,6 @@
     <t>(1) Button 0 and 3</t>
   </si>
   <si>
-    <t>(0) Button 0 and 3</t>
-  </si>
-  <si>
     <t>(1) Button 2</t>
   </si>
   <si>
@@ -120,6 +117,18 @@
   </si>
   <si>
     <t>Production Robot Control Layout</t>
+  </si>
+  <si>
+    <t>Invert Drive</t>
+  </si>
+  <si>
+    <t>Button 9</t>
+  </si>
+  <si>
+    <t>(1) Button 4 and 5</t>
+  </si>
+  <si>
+    <t>(0) Button 0</t>
   </si>
 </sst>
 </file>
@@ -192,8 +201,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D9" totalsRowShown="0">
-  <autoFilter ref="A2:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D10" totalsRowShown="0">
+  <autoFilter ref="A2:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Mechanism"/>
     <tableColumn id="2" name="Port(s)"/>
@@ -501,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +526,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -562,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +599,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,7 +613,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,7 +627,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,10 +638,24 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>30</v>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some fiddling with the invert functions in the entire project, optimized some of the command VI's, and named SwerveTeleop more appropriately.
</commit_message>
<xml_diff>
--- a/Team 34 Code/Robot Control Layout.xlsx
+++ b/Team 34 Code/Robot Control Layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -513,7 +513,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>